<commit_message>
Connecting Eclipse to Tomcat
</commit_message>
<xml_diff>
--- a/me_docs/1.Getting-Started-with-JSP.xlsx
+++ b/me_docs/1.Getting-Started-with-JSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AEE7B6-B10A-43FA-945F-8C52D39CA6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A254FAB-F92E-411E-8199-8306F7576148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="download java" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="jre install" sheetId="3" r:id="rId3"/>
     <sheet name="Installing Tomcat" sheetId="4" r:id="rId4"/>
     <sheet name="Installing Eclipse" sheetId="5" r:id="rId5"/>
+    <sheet name="Tomcat plugin,java for eclipse" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>URL: https://www.oracle.com/java/technologies/javase/javase9-archive-downloads.html</t>
   </si>
@@ -137,6 +138,18 @@
   <si>
     <t>Run eclipse</t>
   </si>
+  <si>
+    <t>Install tomcat plugin from marketplace to eclipse để liên kết tomcat với eclipse</t>
+  </si>
+  <si>
+    <t>サーバー・ランタイム環境の追加(Chỉ định folder tomcat)</t>
+  </si>
+  <si>
+    <t>インストールしたJDKをEclipseに適用する</t>
+  </si>
+  <si>
+    <t>Create ext folder and copy paste jar file</t>
+  </si>
 </sst>
 </file>
 
@@ -1856,6 +1869,759 @@
         <a:xfrm>
           <a:off x="609600" y="25717500"/>
           <a:ext cx="13009524" cy="6961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142095</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>189952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B38BD0-8729-4AE1-8CA0-2CF7BFE6A8FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="6238095" cy="4380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>27581</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>27714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9240EBC-AF7E-409C-994F-D0A91DEC1EB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5143500"/>
+          <a:ext cx="7952381" cy="6885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>18057</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>151548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1191F34F-E439-45DE-8DDE-916104838CF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="12192000"/>
+          <a:ext cx="7942857" cy="6819048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>389943</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>142405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F3AD56-83EA-4B68-A48D-21C3E408C400}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19240500"/>
+          <a:ext cx="4657143" cy="3761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>36495</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>104309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A42BE992-8761-4373-8850-1DB240C57B31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="23431500"/>
+          <a:ext cx="12838095" cy="3723809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542095</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>85071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE9BCE5C-3B61-4BE9-AA27-50E834798676}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="27432000"/>
+          <a:ext cx="6638095" cy="5228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>161238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{376143D0-98F8-44B2-80FD-9FA496E66712}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32956500"/>
+          <a:ext cx="4866667" cy="5495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>570895</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>142190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9136F5-4BA8-4A13-B40F-FBC375DFCA38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="38671500"/>
+          <a:ext cx="4838095" cy="5476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504000</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>66024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5D3022C-A1D3-40E1-A6A3-DFDC885D0776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="44386500"/>
+          <a:ext cx="6600000" cy="5209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>36495</xdr:colOff>
+      <xdr:row>309</xdr:row>
+      <xdr:rowOff>104309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21893983-4163-47DC-BF27-55D38F76C365}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="50101500"/>
+          <a:ext cx="12838095" cy="3723809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>310</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>113448</xdr:colOff>
+      <xdr:row>338</xdr:row>
+      <xdr:rowOff>8857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC5DE93A-A5E8-4759-8D12-178603437BF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="53911500"/>
+          <a:ext cx="6819048" cy="5342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>339</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>361</xdr:row>
+      <xdr:rowOff>75667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAFFF540-C7F6-42C6-BF28-098897079CDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="59436000"/>
+          <a:ext cx="4876190" cy="4266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>227657</xdr:colOff>
+      <xdr:row>287</xdr:row>
+      <xdr:rowOff>132738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03022AF0-9DBB-412A-9FBB-0F32189FE6C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="49911000"/>
+          <a:ext cx="7542857" cy="4895238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>363</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589943</xdr:colOff>
+      <xdr:row>388</xdr:row>
+      <xdr:rowOff>123214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABC76A9B-33DE-460B-8261-8427EDC13CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="69151500"/>
+          <a:ext cx="4857143" cy="4885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>390</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>141714</xdr:colOff>
+      <xdr:row>418</xdr:row>
+      <xdr:rowOff>161238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2306D50-99FF-4D2A-A3EE-2C67613AA386}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="74295000"/>
+          <a:ext cx="9285714" cy="5495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>420</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>589790</xdr:colOff>
+      <xdr:row>453</xdr:row>
+      <xdr:rowOff>151595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00391FAE-19BF-4258-B2AF-FF6A95E52120}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="80010000"/>
+          <a:ext cx="6076190" cy="6438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>455</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>84876</xdr:colOff>
+      <xdr:row>483</xdr:row>
+      <xdr:rowOff>18381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB88DC5B-71A2-4616-B236-C675348A0F29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="86677500"/>
+          <a:ext cx="6790476" cy="5352381"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2199,7 +2965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BC24AF-AE10-4EF2-8A7E-017D29D19140}">
   <dimension ref="A2:B272"/>
   <sheetViews>
-    <sheetView topLeftCell="A295" workbookViewId="0">
+    <sheetView topLeftCell="A157" workbookViewId="0">
       <selection activeCell="B311" sqref="B311"/>
     </sheetView>
   </sheetViews>
@@ -2256,7 +3022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D8C7A4-AEF3-40C9-B4C2-4B47E6114AD5}">
   <dimension ref="A2:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+    <sheetView topLeftCell="A154" workbookViewId="0">
       <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
@@ -2286,4 +3052,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB809D5E-B879-473D-8E37-44DD9B030281}">
+  <dimension ref="A2:A290"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A463" workbookViewId="0">
+      <selection activeCell="K492" sqref="K492"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Deploying To Tomcat using WAR files
</commit_message>
<xml_diff>
--- a/me_docs/1.Getting-Started-with-JSP.xlsx
+++ b/me_docs/1.Getting-Started-with-JSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76413363-AB31-4D71-84CB-78DB527744B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D5B596-2D12-4E7E-BA9C-9C16F250A1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="download java" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>URL: https://www.oracle.com/java/technologies/javase/javase9-archive-downloads.html</t>
   </si>
@@ -176,6 +176,9 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>admin</t>
+  </si>
 </sst>
 </file>
 
@@ -220,12 +223,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,10 +249,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3046,10 +3056,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BC24AF-AE10-4EF2-8A7E-017D29D19140}">
-  <dimension ref="A2:B272"/>
+  <dimension ref="A2:J272"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B311" sqref="B311"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="M136" sqref="M135:M136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,6 +3072,16 @@
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J132" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J133" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3105,7 +3125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D8C7A4-AEF3-40C9-B4C2-4B47E6114AD5}">
   <dimension ref="A2:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
@@ -3141,7 +3161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB809D5E-B879-473D-8E37-44DD9B030281}">
   <dimension ref="A2:B390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A410" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="O384" sqref="O384"/>
     </sheetView>
   </sheetViews>
@@ -3183,7 +3203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8E4FF5-28A0-4289-AF48-A85DEE5715D0}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="T92" sqref="T92"/>
     </sheetView>
   </sheetViews>

</xml_diff>